<commit_message>
in-lab runs, raw iohub records button-box ok
</commit_message>
<xml_diff>
--- a/BLOCKA.xlsx
+++ b/BLOCKA.xlsx
@@ -10,9 +10,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$E$49</definedName>
-  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -252,10 +249,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
   <a:themeElements>
@@ -370,7 +363,7 @@
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1:L1"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1234,7 +1227,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E49"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1242,6 +1234,5 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>